<commit_message>
New data in data.xlsx
</commit_message>
<xml_diff>
--- a/resource/data.xlsx
+++ b/resource/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ba4b54c11903064a/Desktop/Excel Automation/Project/resource/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ba4b54c11903064a/Desktop/Excel Automation/AutomationTestScript/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="11_F25DC773A252ABDACC1048F2591C73145BDE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66622591-60FC-4E71-B5C8-57299FE0A954}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_F25DC773A252ABDACC1048F2591C73145BDE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AC0AE8A-0D22-49ED-B5BC-A855C13B0873}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>Tablename</t>
   </si>
@@ -57,7 +57,22 @@
     <t>SELECT * FROM HR.EMPLOYEES</t>
   </si>
   <si>
-    <t>EMPLOYEES_NEW</t>
+    <t>select * from stg_department</t>
+  </si>
+  <si>
+    <t>select * from stg_employees</t>
+  </si>
+  <si>
+    <t>Department_ID</t>
+  </si>
+  <si>
+    <t>STG_EMPLOYEES</t>
+  </si>
+  <si>
+    <t>DEPARTMENTS</t>
+  </si>
+  <si>
+    <t>SELECT * FROM HR.DEPARTMENTS</t>
   </si>
 </sst>
 </file>
@@ -109,9 +124,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,17 +425,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
@@ -444,8 +457,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -457,13 +470,13 @@
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -474,8 +487,42 @@
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
POC on Excel to Excel comparison with same code
</commit_message>
<xml_diff>
--- a/resource/data.xlsx
+++ b/resource/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ba4b54c11903064a/Desktop/Excel Automation/AutomationTestScript/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_F25DC773A252ABDACC1048F2591C73145BDE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AC0AE8A-0D22-49ED-B5BC-A855C13B0873}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="11_F25DC773A252ABDACC1048F2591C73145BDE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B71D51C-9B0B-4222-8AA9-3D92895EEA74}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,9 +63,6 @@
     <t>select * from stg_employees</t>
   </si>
   <si>
-    <t>Department_ID</t>
-  </si>
-  <si>
     <t>STG_EMPLOYEES</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>SELECT * FROM HR.DEPARTMENTS</t>
+  </si>
+  <si>
+    <t>DEPARTMENT_ID</t>
   </si>
 </sst>
 </file>
@@ -121,10 +121,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -159,6 +158,10 @@
 </file>
 
 <file path=xl/persons/person3.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person4.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -428,7 +431,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -436,7 +439,7 @@
     <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -458,70 +461,70 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>